<commit_message>
add front matter, wrap up all testing
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-ws-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-ws-parsing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80306D49-8415-9847-A6C0-09E79E588592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490FC3AD-4187-7541-A949-04A31EA33D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="2380" windowWidth="16100" windowHeight="17460" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="1620" yWindow="6140" windowWidth="28680" windowHeight="17460" activeTab="2" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
   <si>
     <t>passwordHash</t>
   </si>
@@ -255,6 +255,24 @@
   </si>
   <si>
     <t>key</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>test basic spreadsheet parsing</t>
+  </si>
+  <si>
+    <t>someNumber</t>
+  </si>
+  <si>
+    <t>someBool</t>
+  </si>
+  <si>
+    <t>created</t>
   </si>
 </sst>
 </file>
@@ -319,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -346,6 +364,11 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,310 +699,353 @@
     <col min="7" max="7" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>42</v>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="2">
-        <v>-100</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8">
-        <v>40544</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>53</v>
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="2">
-        <v>9999</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="b">
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="8">
-        <v>44594</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="2">
-        <v>9999</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>44594</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2">
-        <v>15.1515</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="8">
-        <v>12116</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="2">
-        <v>-2000.1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="8">
-        <v>16166</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>61</v>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2">
+        <v>-100</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
+        <v>40544</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2">
+        <v>9999</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="8">
-        <v>20214</v>
-      </c>
-      <c r="F8" s="2">
-        <v>123</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="11">
-        <v>24264</v>
+      <c r="E9" s="8">
+        <v>44594</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>9999</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
+        <v>44594</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="2" t="str">
-        <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>31e41d77-1a31-4fea-8bf2-8fa0a11ee86a</v>
+        <v>51</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="A11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2">
+        <v>15.1515</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="8">
+        <v>12116</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2">
+        <v>-2000.1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="8">
+        <v>16166</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="8">
+        <v>20214</v>
+      </c>
+      <c r="F13" s="2">
+        <v>123</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="11">
+        <v>24264</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="2" t="str">
+        <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
+        <v>3ec8ea13-8140-41e2-a1f8-aa77f880db95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:J2" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:J7" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:H2" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:H7 B2:B4" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
       <formula1>DataTypeList</formula1>
     </dataValidation>
   </dataValidations>
@@ -992,7 +1058,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DFAE23-AEC5-7049-89FE-89CD900ABF71}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1057,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16853B8-B19B-5340-B113-FF91073746DD}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1069,43 +1137,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="14">
+        <v>45542</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="2" t="e">
+      <c r="B6" s="2" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C3" s="2" t="e">
+      <c r="C6" s="2" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:C2" xr:uid="{7E599051-098C-074E-B40E-BBA797C69756}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:C5 B2" xr:uid="{7E599051-098C-074E-B40E-BBA797C69756}">
       <formula1>DataTypeList</formula1>
     </dataValidation>
   </dataValidations>
@@ -1118,7 +1207,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finished arango utils database create + tests
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-parser/tests/test-ws-parsing.xlsx
+++ b/packages/spreadsheet-parser/tests/test-ws-parsing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-parser/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490FC3AD-4187-7541-A949-04A31EA33D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DC9392-F800-C447-92D3-57285131FCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="6140" windowWidth="28680" windowHeight="17460" activeTab="2" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="51100" yWindow="5140" windowWidth="26820" windowHeight="19240" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="H15" s="2" t="str">
         <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
-        <v>3ec8ea13-8140-41e2-a1f8-aa77f880db95</v>
+        <v>7774798a-5b86-4b74-8344-bfee7209bc95</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1127,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16853B8-B19B-5340-B113-FF91073746DD}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>